<commit_message>
2024-04-05 - Borrado de archivos innecesarios
</commit_message>
<xml_diff>
--- a/subidasx/totales_txt_Prueba20240325.xlsx
+++ b/subidasx/totales_txt_Prueba20240325.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="142">
   <si>
     <t>PSTD</t>
   </si>
@@ -82,6 +82,9 @@
     <t>PSTD20240322_030511Cabecera.txt</t>
   </si>
   <si>
+    <t>PSTD20240323_030528Cabecera.txt</t>
+  </si>
+  <si>
     <t xml:space="preserve">Totales : </t>
   </si>
   <si>
@@ -421,10 +424,22 @@
     <t>703</t>
   </si>
   <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>677</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">                                                                                                                </t>
+    <t xml:space="preserve">                                                                                                                         </t>
   </si>
 </sst>
 </file>
@@ -821,7 +836,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -875,7 +890,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>13898566.65</v>
@@ -887,7 +902,7 @@
         <v>50957.84</v>
       </c>
       <c r="F2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G2">
         <f>IF(F2="X",E2,0)</f>
@@ -905,7 +920,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>10442338.7</v>
@@ -917,7 +932,7 @@
         <v>21965.89</v>
       </c>
       <c r="F3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G3">
         <f>IF(F3="X",E3,0)</f>
@@ -935,7 +950,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>9528753.07</v>
@@ -947,7 +962,7 @@
         <v>43699.48</v>
       </c>
       <c r="F4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G4">
         <f>IF(F4="X",E4,0)</f>
@@ -965,7 +980,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>6132577.26</v>
@@ -977,7 +992,7 @@
         <v>39005.36</v>
       </c>
       <c r="F5" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G5">
         <f>IF(F5="X",E5,0)</f>
@@ -995,7 +1010,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>13651265.65</v>
@@ -1007,7 +1022,7 @@
         <v>33017.85</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G6">
         <f>IF(F6="X",E6,0)</f>
@@ -1025,7 +1040,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>17030421.32</v>
@@ -1037,7 +1052,7 @@
         <v>66679.97</v>
       </c>
       <c r="F7" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G7">
         <f>IF(F7="X",E7,0)</f>
@@ -1055,7 +1070,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>13960554.07</v>
@@ -1067,7 +1082,7 @@
         <v>80290.72</v>
       </c>
       <c r="F8" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G8">
         <f>IF(F8="X",E8,0)</f>
@@ -1085,7 +1100,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>10295523.96</v>
@@ -1097,7 +1112,7 @@
         <v>14499.64</v>
       </c>
       <c r="F9" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G9">
         <f>IF(F9="X",E9,0)</f>
@@ -1115,7 +1130,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>12520068.29</v>
@@ -1127,7 +1142,7 @@
         <v>55207.8</v>
       </c>
       <c r="F10" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G10">
         <f>IF(F10="X",E10,0)</f>
@@ -1145,7 +1160,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>10561515.74</v>
@@ -1157,7 +1172,7 @@
         <v>79307.53999999999</v>
       </c>
       <c r="F11" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G11">
         <f>IF(F11="X",E11,0)</f>
@@ -1175,7 +1190,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>4268146.94</v>
@@ -1187,7 +1202,7 @@
         <v>75173.98999999999</v>
       </c>
       <c r="F12" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G12">
         <f>IF(F12="X",E12,0)</f>
@@ -1205,7 +1220,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <v>13546187.51</v>
@@ -1217,7 +1232,7 @@
         <v>73447.69</v>
       </c>
       <c r="F13" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G13">
         <f>IF(F13="X",E13,0)</f>
@@ -1235,7 +1250,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>17442061.9</v>
@@ -1247,7 +1262,7 @@
         <v>119355.79</v>
       </c>
       <c r="F14" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G14">
         <f>IF(F14="X",E14,0)</f>
@@ -1265,7 +1280,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15">
         <v>13486442.82</v>
@@ -1277,7 +1292,7 @@
         <v>33191.50999999999</v>
       </c>
       <c r="F15" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G15">
         <f>IF(F15="X",E15,0)</f>
@@ -1295,7 +1310,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16">
         <v>17386131.84</v>
@@ -1307,7 +1322,7 @@
         <v>62652.07000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G16">
         <f>IF(F16="X",E16,0)</f>
@@ -1325,7 +1340,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17">
         <v>7561876.62</v>
@@ -1337,7 +1352,7 @@
         <v>239837.38</v>
       </c>
       <c r="F17" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G17">
         <f>IF(F17="X",E17,0)</f>
@@ -1355,7 +1370,7 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18">
         <v>14949178.65</v>
@@ -1367,7 +1382,7 @@
         <v>42605.17</v>
       </c>
       <c r="F18" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G18">
         <f>IF(F18="X",E18,0)</f>
@@ -1385,7 +1400,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19">
         <v>12891011.81</v>
@@ -1397,7 +1412,7 @@
         <v>26846.41</v>
       </c>
       <c r="F19" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G19">
         <f>IF(F19="X",E19,0)</f>
@@ -1415,7 +1430,7 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>13088225.08</v>
@@ -1427,7 +1442,7 @@
         <v>33129.88</v>
       </c>
       <c r="F20" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G20">
         <f>IF(F20="X",E20,0)</f>
@@ -1445,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21">
         <v>14933855.52</v>
@@ -1457,7 +1472,7 @@
         <v>46381.07000000001</v>
       </c>
       <c r="F21" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G21">
         <f>IF(F21="X",E21,0)</f>
@@ -1475,7 +1490,7 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C22">
         <v>14982737.58</v>
@@ -1487,7 +1502,7 @@
         <v>34326.88</v>
       </c>
       <c r="F22" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G22">
         <f>IF(F22="X",E22,0)</f>
@@ -1505,7 +1520,7 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23">
         <v>15207712.13</v>
@@ -1517,7 +1532,7 @@
         <v>87977.16</v>
       </c>
       <c r="F23" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G23">
         <f>IF(F23="X",E23,0)</f>
@@ -1535,7 +1550,7 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24">
         <v>9253673.66</v>
@@ -1547,7 +1562,7 @@
         <v>64312.28999999999</v>
       </c>
       <c r="F24" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G24">
         <f>IF(F24="X",E24,0)</f>
@@ -1565,7 +1580,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25">
         <v>7583121.38</v>
@@ -1577,7 +1592,7 @@
         <v>34357.22</v>
       </c>
       <c r="F25" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G25">
         <f>IF(F25="X",E25,0)</f>
@@ -1595,7 +1610,7 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C26">
         <v>10469267.98</v>
@@ -1607,7 +1622,7 @@
         <v>70437.84</v>
       </c>
       <c r="F26" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G26">
         <f>IF(F26="X",E26,0)</f>
@@ -1625,7 +1640,7 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C27">
         <v>9701879.699999999</v>
@@ -1637,7 +1652,7 @@
         <v>35297.89</v>
       </c>
       <c r="F27" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G27">
         <f>IF(F27="X",E27,0)</f>
@@ -1655,7 +1670,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28">
         <v>12797720.74</v>
@@ -1667,7 +1682,7 @@
         <v>43674.52</v>
       </c>
       <c r="F28" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G28">
         <f>IF(F28="X",E28,0)</f>
@@ -1685,7 +1700,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C29">
         <v>15683145.17</v>
@@ -1697,7 +1712,7 @@
         <v>70913.25</v>
       </c>
       <c r="F29" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G29">
         <f>IF(F29="X",E29,0)</f>
@@ -1715,7 +1730,7 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C30">
         <v>9201994.619999999</v>
@@ -1727,7 +1742,7 @@
         <v>49900.7</v>
       </c>
       <c r="F30" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G30">
         <f>IF(F30="X",E30,0)</f>
@@ -1745,7 +1760,7 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C31">
         <v>14087600.26</v>
@@ -1757,7 +1772,7 @@
         <v>7251.53</v>
       </c>
       <c r="F31" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G31">
         <f>IF(F31="X",E31,0)</f>
@@ -1775,7 +1790,7 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C32">
         <v>10403980.64</v>
@@ -1787,7 +1802,7 @@
         <v>51743.97</v>
       </c>
       <c r="F32" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G32">
         <f>IF(F32="X",E32,0)</f>
@@ -1805,7 +1820,7 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C33">
         <v>12646422.34</v>
@@ -1817,7 +1832,7 @@
         <v>62277.34</v>
       </c>
       <c r="F33" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G33">
         <f>IF(F33="X",E33,0)</f>
@@ -1835,7 +1850,7 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C34">
         <v>12185730.87</v>
@@ -1847,7 +1862,7 @@
         <v>33854.84</v>
       </c>
       <c r="F34" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G34">
         <f>IF(F34="X",E34,0)</f>
@@ -1865,7 +1880,7 @@
         <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C35">
         <v>15816218.86</v>
@@ -1877,7 +1892,7 @@
         <v>61436.48</v>
       </c>
       <c r="F35" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G35">
         <f>IF(F35="X",E35,0)</f>
@@ -1895,7 +1910,7 @@
         <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C36">
         <v>18785191.64</v>
@@ -1907,7 +1922,7 @@
         <v>128117.88</v>
       </c>
       <c r="F36" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G36">
         <f>IF(F36="X",E36,0)</f>
@@ -1925,7 +1940,7 @@
         <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C37">
         <v>8235194.8</v>
@@ -1937,7 +1952,7 @@
         <v>15427.62</v>
       </c>
       <c r="F37" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G37">
         <f>IF(F37="X",E37,0)</f>
@@ -1955,7 +1970,7 @@
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C38">
         <v>9489147.709999999</v>
@@ -1967,7 +1982,7 @@
         <v>37293.63</v>
       </c>
       <c r="F38" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G38">
         <f>IF(F38="X",E38,0)</f>
@@ -1985,7 +2000,7 @@
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C39">
         <v>7083318.83</v>
@@ -1997,7 +2012,7 @@
         <v>18037.83</v>
       </c>
       <c r="F39" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G39">
         <f>IF(F39="X",E39,0)</f>
@@ -2015,7 +2030,7 @@
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C40">
         <v>5610174.42</v>
@@ -2027,7 +2042,7 @@
         <v>12325.25</v>
       </c>
       <c r="F40" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G40">
         <f>IF(F40="X",E40,0)</f>
@@ -2045,7 +2060,7 @@
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C41">
         <v>16063511.21</v>
@@ -2057,7 +2072,7 @@
         <v>94499.84</v>
       </c>
       <c r="F41" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G41">
         <f>IF(F41="X",E41,0)</f>
@@ -2075,7 +2090,7 @@
         <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C42">
         <v>13316159.72</v>
@@ -2087,7 +2102,7 @@
         <v>64922.81</v>
       </c>
       <c r="F42" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G42">
         <f>IF(F42="X",E42,0)</f>
@@ -2105,7 +2120,7 @@
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C43">
         <v>11368462.49</v>
@@ -2117,7 +2132,7 @@
         <v>52209.67</v>
       </c>
       <c r="F43" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G43">
         <f>IF(F43="X",E43,0)</f>
@@ -2135,7 +2150,7 @@
         <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C44">
         <v>16009340.87</v>
@@ -2147,7 +2162,7 @@
         <v>63777.15</v>
       </c>
       <c r="F44" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G44">
         <f>IF(F44="X",E44,0)</f>
@@ -2165,7 +2180,7 @@
         <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C45">
         <v>10294637.74</v>
@@ -2177,7 +2192,7 @@
         <v>28551.66</v>
       </c>
       <c r="F45" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G45">
         <f>IF(F45="X",E45,0)</f>
@@ -2195,7 +2210,7 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C46">
         <v>15018033.03</v>
@@ -2207,7 +2222,7 @@
         <v>66887.34000000001</v>
       </c>
       <c r="F46" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G46">
         <f>IF(F46="X",E46,0)</f>
@@ -2225,7 +2240,7 @@
         <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C47">
         <v>11616336.24</v>
@@ -2237,7 +2252,7 @@
         <v>51820.24000000001</v>
       </c>
       <c r="F47" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G47">
         <f>IF(F47="X",E47,0)</f>
@@ -2255,7 +2270,7 @@
         <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C48">
         <v>19791193.17</v>
@@ -2267,7 +2282,7 @@
         <v>64987.89999999999</v>
       </c>
       <c r="F48" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G48">
         <f>IF(F48="X",E48,0)</f>
@@ -2285,7 +2300,7 @@
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C49">
         <v>272210.15</v>
@@ -2297,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G49">
         <f>IF(F49="X",E49,0)</f>
@@ -2315,7 +2330,7 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C50">
         <v>8247442.36</v>
@@ -2327,7 +2342,7 @@
         <v>14454.14</v>
       </c>
       <c r="F50" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G50">
         <f>IF(F50="X",E50,0)</f>
@@ -2345,7 +2360,7 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C51">
         <v>7480979.28</v>
@@ -2357,7 +2372,7 @@
         <v>85726.53</v>
       </c>
       <c r="F51" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G51">
         <f>IF(F51="X",E51,0)</f>
@@ -2375,7 +2390,7 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C52">
         <v>14300497.21</v>
@@ -2387,7 +2402,7 @@
         <v>32384.37</v>
       </c>
       <c r="F52" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G52">
         <f>IF(F52="X",E52,0)</f>
@@ -2405,7 +2420,7 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C53">
         <v>15758605.88</v>
@@ -2417,7 +2432,7 @@
         <v>72993.23</v>
       </c>
       <c r="F53" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G53">
         <f>IF(F53="X",E53,0)</f>
@@ -2435,7 +2450,7 @@
         <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C54">
         <v>14897103.41</v>
@@ -2447,7 +2462,7 @@
         <v>83249.78999999999</v>
       </c>
       <c r="F54" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G54">
         <f>IF(F54="X",E54,0)</f>
@@ -2465,7 +2480,7 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C55">
         <v>9231312.18</v>
@@ -2477,7 +2492,7 @@
         <v>32278.24</v>
       </c>
       <c r="F55" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G55">
         <f>IF(F55="X",E55,0)</f>
@@ -2495,7 +2510,7 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C56">
         <v>11858084.32</v>
@@ -2507,7 +2522,7 @@
         <v>48671.92</v>
       </c>
       <c r="F56" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G56">
         <f>IF(F56="X",E56,0)</f>
@@ -2525,7 +2540,7 @@
         <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C57">
         <v>20866061.96</v>
@@ -2537,7 +2552,7 @@
         <v>237850.78</v>
       </c>
       <c r="F57" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G57">
         <f>IF(F57="X",E57,0)</f>
@@ -2555,7 +2570,7 @@
         <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C58">
         <v>15828087.37</v>
@@ -2567,7 +2582,7 @@
         <v>38597.39</v>
       </c>
       <c r="F58" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G58">
         <f>IF(F58="X",E58,0)</f>
@@ -2585,7 +2600,7 @@
         <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C59">
         <v>14634949.2</v>
@@ -2597,7 +2612,7 @@
         <v>60665.52</v>
       </c>
       <c r="F59" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G59">
         <f>IF(F59="X",E59,0)</f>
@@ -2615,7 +2630,7 @@
         <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C60">
         <v>11327493.38</v>
@@ -2627,7 +2642,7 @@
         <v>16401.07</v>
       </c>
       <c r="F60" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G60">
         <f>IF(F60="X",E60,0)</f>
@@ -2645,7 +2660,7 @@
         <v>14</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C61">
         <v>12267220.35</v>
@@ -2657,7 +2672,7 @@
         <v>24102.62</v>
       </c>
       <c r="F61" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G61">
         <f>IF(F61="X",E61,0)</f>
@@ -2675,7 +2690,7 @@
         <v>15</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C62">
         <v>10145261.22</v>
@@ -2687,7 +2702,7 @@
         <v>53783.81999999999</v>
       </c>
       <c r="F62" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G62">
         <f>IF(F62="X",E62,0)</f>
@@ -2705,7 +2720,7 @@
         <v>15</v>
       </c>
       <c r="B63" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C63">
         <v>9326781.529999999</v>
@@ -2717,7 +2732,7 @@
         <v>64622.96999999999</v>
       </c>
       <c r="F63" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G63">
         <f>IF(F63="X",E63,0)</f>
@@ -2735,7 +2750,7 @@
         <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C64">
         <v>13676551.79</v>
@@ -2747,7 +2762,7 @@
         <v>35294.01</v>
       </c>
       <c r="F64" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G64">
         <f>IF(F64="X",E64,0)</f>
@@ -2765,7 +2780,7 @@
         <v>15</v>
       </c>
       <c r="B65" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C65">
         <v>8913384.59</v>
@@ -2777,7 +2792,7 @@
         <v>7564.11</v>
       </c>
       <c r="F65" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G65">
         <f>IF(F65="X",E65,0)</f>
@@ -2795,7 +2810,7 @@
         <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C66">
         <v>15129943.63</v>
@@ -2807,7 +2822,7 @@
         <v>60333.36</v>
       </c>
       <c r="F66" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G66">
         <f>IF(F66="X",E66,0)</f>
@@ -2825,7 +2840,7 @@
         <v>15</v>
       </c>
       <c r="B67" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C67">
         <v>8593443.029999999</v>
@@ -2837,7 +2852,7 @@
         <v>31330.18</v>
       </c>
       <c r="F67" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G67">
         <f>IF(F67="X",E67,0)</f>
@@ -2855,7 +2870,7 @@
         <v>15</v>
       </c>
       <c r="B68" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C68">
         <v>9328360.939999999</v>
@@ -2867,7 +2882,7 @@
         <v>37676.25</v>
       </c>
       <c r="F68" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G68">
         <f>IF(F68="X",E68,0)</f>
@@ -2885,7 +2900,7 @@
         <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C69">
         <v>17504558.68</v>
@@ -2897,7 +2912,7 @@
         <v>203629.96</v>
       </c>
       <c r="F69" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G69">
         <f>IF(F69="X",E69,0)</f>
@@ -2915,7 +2930,7 @@
         <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C70">
         <v>11114272.06</v>
@@ -2927,7 +2942,7 @@
         <v>20415.74</v>
       </c>
       <c r="F70" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G70">
         <f>IF(F70="X",E70,0)</f>
@@ -2945,7 +2960,7 @@
         <v>16</v>
       </c>
       <c r="B71" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C71">
         <v>12122472.24</v>
@@ -2957,7 +2972,7 @@
         <v>42508.35000000001</v>
       </c>
       <c r="F71" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G71">
         <f>IF(F71="X",E71,0)</f>
@@ -2975,7 +2990,7 @@
         <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C72">
         <v>16178229.95</v>
@@ -2987,7 +3002,7 @@
         <v>101843.34</v>
       </c>
       <c r="F72" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G72">
         <f>IF(F72="X",E72,0)</f>
@@ -3005,7 +3020,7 @@
         <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C73">
         <v>5647996.66</v>
@@ -3017,7 +3032,7 @@
         <v>13782.51</v>
       </c>
       <c r="F73" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G73">
         <f>IF(F73="X",E73,0)</f>
@@ -3035,7 +3050,7 @@
         <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C74">
         <v>8616517.800000001</v>
@@ -3047,7 +3062,7 @@
         <v>27142.36</v>
       </c>
       <c r="F74" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G74">
         <f>IF(F74="X",E74,0)</f>
@@ -3065,7 +3080,7 @@
         <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C75">
         <v>16668236.09</v>
@@ -3077,7 +3092,7 @@
         <v>442632.73</v>
       </c>
       <c r="F75" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G75">
         <f>IF(F75="X",E75,0)</f>
@@ -3095,7 +3110,7 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C76">
         <v>10685142.17</v>
@@ -3107,7 +3122,7 @@
         <v>54292.09</v>
       </c>
       <c r="F76" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G76">
         <f>IF(F76="X",E76,0)</f>
@@ -3125,7 +3140,7 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C77">
         <v>8253420.32</v>
@@ -3137,7 +3152,7 @@
         <v>33960.47</v>
       </c>
       <c r="F77" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G77">
         <f>IF(F77="X",E77,0)</f>
@@ -3155,7 +3170,7 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C78">
         <v>9703706.27</v>
@@ -3167,7 +3182,7 @@
         <v>27174.65</v>
       </c>
       <c r="F78" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G78">
         <f>IF(F78="X",E78,0)</f>
@@ -3185,7 +3200,7 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C79">
         <v>13904137.49</v>
@@ -3197,7 +3212,7 @@
         <v>13569.72</v>
       </c>
       <c r="F79" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G79">
         <f>IF(F79="X",E79,0)</f>
@@ -3215,7 +3230,7 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C80">
         <v>11634587.97</v>
@@ -3227,7 +3242,7 @@
         <v>13419.04</v>
       </c>
       <c r="F80" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G80">
         <f>IF(F80="X",E80,0)</f>
@@ -3245,7 +3260,7 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C81">
         <v>20588217.7</v>
@@ -3257,7 +3272,7 @@
         <v>13580.48</v>
       </c>
       <c r="F81" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G81">
         <f>IF(F81="X",E81,0)</f>
@@ -3275,7 +3290,7 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C82">
         <v>10195187.6</v>
@@ -3287,7 +3302,7 @@
         <v>20476.87</v>
       </c>
       <c r="F82" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G82">
         <f>IF(F82="X",E82,0)</f>
@@ -3305,7 +3320,7 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C83">
         <v>15851907.64</v>
@@ -3317,7 +3332,7 @@
         <v>47699.46999999999</v>
       </c>
       <c r="F83" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G83">
         <f>IF(F83="X",E83,0)</f>
@@ -3335,7 +3350,7 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C84">
         <v>18447077.36</v>
@@ -3347,7 +3362,7 @@
         <v>34483.89</v>
       </c>
       <c r="F84" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G84">
         <f>IF(F84="X",E84,0)</f>
@@ -3365,7 +3380,7 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C85">
         <v>12331685.19</v>
@@ -3377,7 +3392,7 @@
         <v>221353.32</v>
       </c>
       <c r="F85" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G85">
         <f>IF(F85="X",E85,0)</f>
@@ -3395,7 +3410,7 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C86">
         <v>12056584.91</v>
@@ -3407,7 +3422,7 @@
         <v>145370.68</v>
       </c>
       <c r="F86" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G86">
         <f>IF(F86="X",E86,0)</f>
@@ -3425,7 +3440,7 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C87">
         <v>11458681.18</v>
@@ -3437,7 +3452,7 @@
         <v>102440.16</v>
       </c>
       <c r="F87" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G87">
         <f>IF(F87="X",E87,0)</f>
@@ -3455,7 +3470,7 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C88">
         <v>16134884.81</v>
@@ -3467,7 +3482,7 @@
         <v>47406.45</v>
       </c>
       <c r="F88" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G88">
         <f>IF(F88="X",E88,0)</f>
@@ -3485,7 +3500,7 @@
         <v>18</v>
       </c>
       <c r="B89" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C89">
         <v>15037973.28</v>
@@ -3497,7 +3512,7 @@
         <v>34022.14</v>
       </c>
       <c r="F89" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G89">
         <f>IF(F89="X",E89,0)</f>
@@ -3515,7 +3530,7 @@
         <v>18</v>
       </c>
       <c r="B90" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C90">
         <v>20637212.99</v>
@@ -3527,7 +3542,7 @@
         <v>74777.73</v>
       </c>
       <c r="F90" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G90">
         <f>IF(F90="X",E90,0)</f>
@@ -3545,7 +3560,7 @@
         <v>18</v>
       </c>
       <c r="B91" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C91">
         <v>25855747.91</v>
@@ -3557,7 +3572,7 @@
         <v>75208.74000000001</v>
       </c>
       <c r="F91" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G91">
         <f>IF(F91="X",E91,0)</f>
@@ -3575,7 +3590,7 @@
         <v>18</v>
       </c>
       <c r="B92" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C92">
         <v>11824797.71</v>
@@ -3587,7 +3602,7 @@
         <v>20467.08</v>
       </c>
       <c r="F92" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G92">
         <f>IF(F92="X",E92,0)</f>
@@ -3605,7 +3620,7 @@
         <v>18</v>
       </c>
       <c r="B93" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C93">
         <v>11166565.05</v>
@@ -3617,7 +3632,7 @@
         <v>6776.05</v>
       </c>
       <c r="F93" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G93">
         <f>IF(F93="X",E93,0)</f>
@@ -3635,7 +3650,7 @@
         <v>18</v>
       </c>
       <c r="B94" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C94">
         <v>10683715.61</v>
@@ -3647,7 +3662,7 @@
         <v>20352.62</v>
       </c>
       <c r="F94" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G94">
         <f>IF(F94="X",E94,0)</f>
@@ -3665,7 +3680,7 @@
         <v>18</v>
       </c>
       <c r="B95" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C95">
         <v>21074054.85</v>
@@ -3677,7 +3692,7 @@
         <v>68050.60000000001</v>
       </c>
       <c r="F95" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G95">
         <f>IF(F95="X",E95,0)</f>
@@ -3695,7 +3710,7 @@
         <v>18</v>
       </c>
       <c r="B96" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C96">
         <v>21765190.86</v>
@@ -3707,7 +3722,7 @@
         <v>34030.45</v>
       </c>
       <c r="F96" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G96">
         <f>IF(F96="X",E96,0)</f>
@@ -3725,7 +3740,7 @@
         <v>18</v>
       </c>
       <c r="B97" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C97">
         <v>22171005.57</v>
@@ -3737,7 +3752,7 @@
         <v>33722.27</v>
       </c>
       <c r="F97" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G97">
         <f>IF(F97="X",E97,0)</f>
@@ -3755,7 +3770,7 @@
         <v>18</v>
       </c>
       <c r="B98" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C98">
         <v>13499186.56</v>
@@ -3767,7 +3782,7 @@
         <v>40925.35000000001</v>
       </c>
       <c r="F98" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G98">
         <f>IF(F98="X",E98,0)</f>
@@ -3785,7 +3800,7 @@
         <v>19</v>
       </c>
       <c r="B99" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C99">
         <v>9448351.800000001</v>
@@ -3797,7 +3812,7 @@
         <v>27212.34</v>
       </c>
       <c r="F99" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G99">
         <f>IF(F99="X",E99,0)</f>
@@ -3815,7 +3830,7 @@
         <v>19</v>
       </c>
       <c r="B100" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C100">
         <v>24349990.38</v>
@@ -3827,7 +3842,7 @@
         <v>61292.18</v>
       </c>
       <c r="F100" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G100">
         <f>IF(F100="X",E100,0)</f>
@@ -3845,7 +3860,7 @@
         <v>19</v>
       </c>
       <c r="B101" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C101">
         <v>14588567.59</v>
@@ -3857,7 +3872,7 @@
         <v>13451.81</v>
       </c>
       <c r="F101" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G101">
         <f>IF(F101="X",E101,0)</f>
@@ -3875,7 +3890,7 @@
         <v>20</v>
       </c>
       <c r="B102" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C102">
         <v>12620738.12</v>
@@ -3887,7 +3902,7 @@
         <v>326491.32</v>
       </c>
       <c r="F102" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G102">
         <f>IF(F102="X",E102,0)</f>
@@ -3905,7 +3920,7 @@
         <v>20</v>
       </c>
       <c r="B103" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C103">
         <v>16962810.92</v>
@@ -3917,7 +3932,7 @@
         <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G103">
         <f>IF(F103="X",E103,0)</f>
@@ -3935,7 +3950,7 @@
         <v>20</v>
       </c>
       <c r="B104" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C104">
         <v>18670378.31</v>
@@ -3947,7 +3962,7 @@
         <v>0</v>
       </c>
       <c r="F104" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G104">
         <f>IF(F104="X",E104,0)</f>
@@ -3965,7 +3980,7 @@
         <v>20</v>
       </c>
       <c r="B105" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C105">
         <v>13535083.48</v>
@@ -3977,7 +3992,7 @@
         <v>0</v>
       </c>
       <c r="F105" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G105">
         <f>IF(F105="X",E105,0)</f>
@@ -3995,7 +4010,7 @@
         <v>20</v>
       </c>
       <c r="B106" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C106">
         <v>13033718.6</v>
@@ -4007,7 +4022,7 @@
         <v>0</v>
       </c>
       <c r="F106" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G106">
         <f>IF(F106="X",E106,0)</f>
@@ -4025,7 +4040,7 @@
         <v>20</v>
       </c>
       <c r="B107" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C107">
         <v>15696068.85</v>
@@ -4037,7 +4052,7 @@
         <v>407034.98</v>
       </c>
       <c r="F107" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G107">
         <f>IF(F107="X",E107,0)</f>
@@ -4055,7 +4070,7 @@
         <v>20</v>
       </c>
       <c r="B108" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C108">
         <v>14104344.68</v>
@@ -4067,7 +4082,7 @@
         <v>0</v>
       </c>
       <c r="F108" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G108">
         <f>IF(F108="X",E108,0)</f>
@@ -4085,7 +4100,7 @@
         <v>20</v>
       </c>
       <c r="B109" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C109">
         <v>17581820.71</v>
@@ -4097,7 +4112,7 @@
         <v>0</v>
       </c>
       <c r="F109" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G109">
         <f>IF(F109="X",E109,0)</f>
@@ -4115,7 +4130,7 @@
         <v>20</v>
       </c>
       <c r="B110" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C110">
         <v>22548495.65</v>
@@ -4127,7 +4142,7 @@
         <v>0</v>
       </c>
       <c r="F110" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G110">
         <f>IF(F110="X",E110,0)</f>
@@ -4145,7 +4160,7 @@
         <v>20</v>
       </c>
       <c r="B111" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C111">
         <v>10839257.73</v>
@@ -4157,7 +4172,7 @@
         <v>0</v>
       </c>
       <c r="F111" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G111">
         <f>IF(F111="X",E111,0)</f>
@@ -4175,7 +4190,7 @@
         <v>20</v>
       </c>
       <c r="B112" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C112">
         <v>19407856.34</v>
@@ -4187,7 +4202,7 @@
         <v>536169.84</v>
       </c>
       <c r="F112" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G112">
         <f>IF(F112="X",E112,0)</f>
@@ -4205,7 +4220,7 @@
         <v>21</v>
       </c>
       <c r="B113" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C113">
         <v>18044155.83</v>
@@ -4217,7 +4232,7 @@
         <v>583168.47</v>
       </c>
       <c r="F113" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G113">
         <f>IF(F113="X",E113,0)</f>
@@ -4234,34 +4249,304 @@
       <c r="A114" t="s">
         <v>22</v>
       </c>
-      <c r="B114">
-        <v>112</v>
+      <c r="B114" t="s">
+        <v>25</v>
       </c>
       <c r="C114">
-        <v>1486604978.45</v>
+        <v>14175567.34</v>
       </c>
       <c r="D114">
-        <v>1163169226.86</v>
+        <v>12693040.23</v>
       </c>
       <c r="E114">
-        <v>7672190.33</v>
+        <v>0</v>
       </c>
       <c r="F114" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G114">
-        <f>SUM(G2:G112)</f>
-        <v>0</v>
-      </c>
-      <c r="H114" t="s">
-        <v>135</v>
-      </c>
-      <c r="I114" t="s">
-        <v>135</v>
+        <f>IF(F114="X",E114,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>20240323</v>
+      </c>
+      <c r="I114">
+        <v>89.54167353981897</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>22</v>
+      </c>
+      <c r="B115" t="s">
+        <v>136</v>
+      </c>
+      <c r="C115">
+        <v>31928909.52</v>
+      </c>
+      <c r="D115">
+        <v>31941545.16</v>
+      </c>
+      <c r="E115">
+        <v>346121.27</v>
+      </c>
+      <c r="F115" t="s">
+        <v>140</v>
+      </c>
+      <c r="G115">
+        <f>IF(F115="X",E115,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>20240323</v>
+      </c>
+      <c r="I115">
+        <v>100.0395742923575</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" t="s">
+        <v>22</v>
+      </c>
+      <c r="B116" t="s">
+        <v>137</v>
+      </c>
+      <c r="C116">
+        <v>26627239.39</v>
+      </c>
+      <c r="D116">
+        <v>26556635.74</v>
+      </c>
+      <c r="E116">
+        <v>360840.88</v>
+      </c>
+      <c r="F116" t="s">
+        <v>140</v>
+      </c>
+      <c r="G116">
+        <f>IF(F116="X",E116,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H116">
+        <v>20240323</v>
+      </c>
+      <c r="I116">
+        <v>99.73484427369321</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
+        <v>22</v>
+      </c>
+      <c r="B117" t="s">
+        <v>138</v>
+      </c>
+      <c r="C117">
+        <v>21842736.44</v>
+      </c>
+      <c r="D117">
+        <v>17704118.12</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117" t="s">
+        <v>140</v>
+      </c>
+      <c r="G117">
+        <f>IF(F117="X",E117,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <v>20240323</v>
+      </c>
+      <c r="I117">
+        <v>81.0526564225668</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" t="s">
+        <v>22</v>
+      </c>
+      <c r="B118" t="s">
+        <v>28</v>
+      </c>
+      <c r="C118">
+        <v>19035510.88</v>
+      </c>
+      <c r="D118">
+        <v>16243409.61</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118" t="s">
+        <v>140</v>
+      </c>
+      <c r="G118">
+        <f>IF(F118="X",E118,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H118">
+        <v>20240323</v>
+      </c>
+      <c r="I118">
+        <v>85.33214428758215</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119" t="s">
+        <v>22</v>
+      </c>
+      <c r="B119" t="s">
+        <v>30</v>
+      </c>
+      <c r="C119">
+        <v>20713987.91</v>
+      </c>
+      <c r="D119">
+        <v>16861272.85</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119" t="s">
+        <v>140</v>
+      </c>
+      <c r="G119">
+        <f>IF(F119="X",E119,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>20240323</v>
+      </c>
+      <c r="I119">
+        <v>81.40041851554794</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" t="s">
+        <v>22</v>
+      </c>
+      <c r="B120" t="s">
+        <v>31</v>
+      </c>
+      <c r="C120">
+        <v>14324239.62</v>
+      </c>
+      <c r="D120">
+        <v>12768512.2</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120" t="s">
+        <v>140</v>
+      </c>
+      <c r="G120">
+        <f>IF(F120="X",E120,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>20240323</v>
+      </c>
+      <c r="I120">
+        <v>89.13919718413646</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
+        <v>22</v>
+      </c>
+      <c r="B121" t="s">
+        <v>32</v>
+      </c>
+      <c r="C121">
+        <v>19021539.18</v>
+      </c>
+      <c r="D121">
+        <v>16193329.78</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121" t="s">
+        <v>140</v>
+      </c>
+      <c r="G121">
+        <f>IF(F121="X",E121,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H121">
+        <v>20240323</v>
+      </c>
+      <c r="I121">
+        <v>85.13154286182218</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" t="s">
+        <v>22</v>
+      </c>
+      <c r="B122" t="s">
+        <v>139</v>
+      </c>
+      <c r="C122">
+        <v>9390643.15</v>
+      </c>
+      <c r="D122">
+        <v>7931360.9</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122" t="s">
+        <v>140</v>
+      </c>
+      <c r="G122">
+        <f>IF(F122="X",E122,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H122">
+        <v>20240323</v>
+      </c>
+      <c r="I122">
+        <v>84.46025233106637</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" t="s">
+        <v>23</v>
+      </c>
+      <c r="B123">
+        <v>121</v>
+      </c>
+      <c r="C123">
+        <v>1663665351.88</v>
+      </c>
+      <c r="D123">
+        <v>1322062451.45</v>
+      </c>
+      <c r="E123">
+        <v>8379152.48</v>
+      </c>
+      <c r="F123" t="s">
+        <v>140</v>
+      </c>
+      <c r="G123">
+        <f>SUM(G2:G121)</f>
+        <v>0</v>
+      </c>
+      <c r="H123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I123" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B112">
+  <conditionalFormatting sqref="B1:B121">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4273,7 +4558,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E112">
+  <conditionalFormatting sqref="E1:E121">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -4281,7 +4566,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H113">
+  <conditionalFormatting sqref="H2:H122">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4293,7 +4578,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I112">
+  <conditionalFormatting sqref="I1:I121">
     <cfRule type="cellIs" dxfId="2" priority="5" operator="between">
       <formula>99</formula>
       <formula>101</formula>

</xml_diff>